<commit_message>
upload file and save
</commit_message>
<xml_diff>
--- a/doc/database.xlsx
+++ b/doc/database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KUJO JOTARO\Desktop\github\nest-bs\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A2450C-B7B4-4BF9-A15B-980C468DF834}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8858CD6F-87B8-4CA5-939A-4BFA9D53C3FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9E1DD6AB-21D5-4F64-B824-AD98C978794E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="98">
   <si>
     <t>mail</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -260,10 +260,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>dislike</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>article_comment</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -417,14 +413,6 @@
   </si>
   <si>
     <t>user_type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>is_like</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0是dislike, 1是like</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -812,10 +800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E846C2B-FA2E-491D-B688-FF85BC6C8EAA}">
-  <dimension ref="A1:G179"/>
+  <dimension ref="A1:G177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -916,7 +904,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -935,10 +923,10 @@
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="F9" s="1"/>
     </row>
@@ -1079,7 +1067,7 @@
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>21</v>
@@ -1094,7 +1082,7 @@
         <v>30</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D23" t="s">
         <v>11</v>
@@ -1139,7 +1127,7 @@
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>24</v>
@@ -1151,7 +1139,7 @@
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>21</v>
@@ -1207,7 +1195,7 @@
         <v>7</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E33" t="s">
         <v>12</v>
@@ -1223,14 +1211,14 @@
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C35" s="1"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C36" s="1"/>
     </row>
@@ -1266,10 +1254,10 @@
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" t="s">
+        <v>74</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="G40">
         <v>0</v>
@@ -1283,7 +1271,7 @@
         <v>7</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E41" t="s">
         <v>12</v>
@@ -1298,16 +1286,16 @@
         <v>1</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" t="s">
+        <v>83</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -1331,28 +1319,28 @@
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" t="s">
+        <v>88</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1370,7 +1358,7 @@
         <v>7</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E50" t="s">
         <v>12</v>
@@ -1414,7 +1402,7 @@
         <v>37</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D54" t="s">
         <v>10</v>
@@ -1483,18 +1471,18 @@
         <v>39</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B63" t="s">
         <v>7</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E63" t="s">
         <v>12</v>
@@ -1506,7 +1494,7 @@
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C64" s="1"/>
     </row>
@@ -1566,19 +1554,21 @@
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
       <c r="B71" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C71" s="1"/>
       <c r="G71">
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4"/>
       <c r="B72" t="s">
-        <v>61</v>
-      </c>
-      <c r="C72" s="1"/>
+        <v>95</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="G72">
         <v>0</v>
       </c>
@@ -1586,55 +1576,50 @@
     <row r="73" spans="1:7" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
       <c r="B73" t="s">
-        <v>96</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G73">
-        <v>0</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="C73" s="1"/>
     </row>
     <row r="74" spans="1:7" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
       <c r="B74" t="s">
-        <v>39</v>
-      </c>
-      <c r="C74" s="1"/>
-    </row>
-    <row r="75" spans="1:7" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
+        <v>57</v>
+      </c>
       <c r="B75" t="s">
-        <v>99</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>100</v>
+        <v>7</v>
+      </c>
+      <c r="C75" s="1"/>
+      <c r="E75" t="s">
+        <v>49</v>
+      </c>
+      <c r="F75" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="4" t="s">
-        <v>58</v>
-      </c>
+      <c r="A76" s="4"/>
       <c r="B76" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="C76" s="1"/>
       <c r="E76" t="s">
-        <v>49</v>
-      </c>
-      <c r="F76" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
       <c r="B77" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="C77" s="1"/>
-      <c r="E77" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
@@ -1646,142 +1631,132 @@
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
       <c r="B79" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="C79" s="1"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
       <c r="B80" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C80" s="1"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="4"/>
+      <c r="A81" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="B81" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="C81" s="1"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="4" t="s">
-        <v>62</v>
-      </c>
+      <c r="A82" s="4"/>
       <c r="B82" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="C82" s="1"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
       <c r="B83" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="C83" s="1"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="4"/>
+      <c r="A84" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="B84" t="s">
-        <v>59</v>
-      </c>
-      <c r="C84" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E84" t="s">
+        <v>12</v>
+      </c>
+      <c r="F84" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="4"/>
       <c r="B85" t="s">
-        <v>97</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>98</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C85" s="1"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="4" t="s">
-        <v>63</v>
-      </c>
+      <c r="A86" s="4"/>
       <c r="B86" t="s">
-        <v>7</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E86" t="s">
-        <v>12</v>
-      </c>
-      <c r="F86" t="s">
-        <v>12</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="C86" s="1"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
       <c r="B87" t="s">
-        <v>1</v>
-      </c>
-      <c r="C87" s="1"/>
+        <v>63</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
       <c r="B88" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C88" s="1"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
       <c r="B89" t="s">
-        <v>64</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>65</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C89" s="1"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
       <c r="B90" t="s">
-        <v>23</v>
-      </c>
-      <c r="C90" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G90" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
       <c r="B91" t="s">
-        <v>29</v>
-      </c>
-      <c r="C91" s="1"/>
+        <v>69</v>
+      </c>
+      <c r="C91" s="5"/>
+      <c r="D91" s="4"/>
+      <c r="G91" s="4"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="4"/>
       <c r="B92" t="s">
         <v>71</v>
       </c>
-      <c r="C92" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D92" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G92" s="4">
-        <v>0</v>
-      </c>
+      <c r="C92" s="5"/>
+      <c r="D92" s="4"/>
+      <c r="G92" s="4"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="4"/>
-      <c r="B93" t="s">
-        <v>70</v>
-      </c>
-      <c r="C93" s="5"/>
-      <c r="D93" s="4"/>
-      <c r="G93" s="4"/>
+      <c r="C93" s="1"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="4"/>
-      <c r="B94" t="s">
-        <v>72</v>
-      </c>
-      <c r="C94" s="5"/>
-      <c r="D94" s="4"/>
-      <c r="G94" s="4"/>
+      <c r="C94" s="1"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C95" s="1"/>
@@ -2032,33 +2007,27 @@
     <row r="177" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C177" s="1"/>
     </row>
-    <row r="178" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C178" s="1"/>
-    </row>
-    <row r="179" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C179" s="1"/>
-    </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="A63:A66"/>
+    <mergeCell ref="C90:C92"/>
+    <mergeCell ref="A84:A92"/>
+    <mergeCell ref="D90:D92"/>
+    <mergeCell ref="G90:G92"/>
+    <mergeCell ref="A75:A80"/>
+    <mergeCell ref="A81:A83"/>
+    <mergeCell ref="A67:A74"/>
     <mergeCell ref="A53:A57"/>
     <mergeCell ref="A25:A32"/>
     <mergeCell ref="A58:A62"/>
     <mergeCell ref="A37:A40"/>
     <mergeCell ref="A41:A48"/>
     <mergeCell ref="A50:A52"/>
-    <mergeCell ref="A63:A66"/>
-    <mergeCell ref="C92:C94"/>
-    <mergeCell ref="A86:A94"/>
-    <mergeCell ref="D92:D94"/>
-    <mergeCell ref="G92:G94"/>
-    <mergeCell ref="A76:A81"/>
-    <mergeCell ref="A67:A75"/>
-    <mergeCell ref="A82:A85"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A33:A36"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>